<commit_message>
get test case running
</commit_message>
<xml_diff>
--- a/__tests__/component/update_student_sheets/test_cases/simple_case/teacher.xlsx
+++ b/__tests__/component/update_student_sheets/test_cases/simple_case/teacher.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsha\Documents\Git\student-teacher-gradebook\__tests__\component\update_student_sheets\test_cases\no_update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsha\Documents\Git\student-teacher-gradebook\__tests__\component\update_student_sheets\test_cases\simple_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A860DE1-2CDE-442F-82DC-03CC65FC5FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3907F-E1BA-403B-B498-88200A6994FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{1C66C71B-6ED8-4699-9FB2-CB3156D48D4F}"/>
+    <workbookView xWindow="-28920" yWindow="1725" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1C66C71B-6ED8-4699-9FB2-CB3156D48D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Student</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Mus476_Stephen Jane_gradebook.xlsx</t>
+  </si>
+  <si>
+    <t>10/10</t>
   </si>
 </sst>
 </file>
@@ -129,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BD79E6-C759-4AA3-AE66-326FEBA345D6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -499,7 +503,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,12 +579,43 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876F72B6-B476-4551-93FD-7FEC013DA096}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>